<commit_message>
Added 84 entries from form (5/20 13:09)
</commit_message>
<xml_diff>
--- a/data/persona-5-questions.xlsx
+++ b/data/persona-5-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joyce\Documents\GitHub\persona5-negotiation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C73CAD-09E5-49D1-8CE4-2D88555EFEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57AD7F7-97FC-4004-8055-837CB2064B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5766" yWindow="1272" windowWidth="17274" windowHeight="11088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14100" yWindow="1650" windowWidth="16398" windowHeight="11088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="1198">
   <si>
     <t>Flag</t>
   </si>
@@ -2801,9 +2801,6 @@
     <t>Skadi, Rangda</t>
   </si>
   <si>
-    <t>Berith, Koropokguru, Oni, Belphegor, Kumbhanda, Hanuman</t>
-  </si>
-  <si>
     <t>Power, Dominion</t>
   </si>
   <si>
@@ -3167,9 +3164,6 @@
     <t>Agathion, Onmoraki, Kodama</t>
   </si>
   <si>
-    <t>Mandrake, Angel, Lilim</t>
-  </si>
-  <si>
     <t>Norn, Scathach, High Pixie, Sarasvati, Silky, Parvati, Queen Mab, Lamia, Leanan Sidhe, Apsaras, Valkyrie</t>
   </si>
   <si>
@@ -3323,12 +3317,6 @@
     <t>Queen Mab, Leanan Sidhe, Silky, Apsaras, Isis, Lamia</t>
   </si>
   <si>
-    <t>Mandrake, Succubus, Lilim</t>
-  </si>
-  <si>
-    <t>Succubus, Angel, Mandrake</t>
-  </si>
-  <si>
     <t>Baphomet, Bicorn, Choronzon, Ippon-Datara, Forneus, Belphegor, Anubis, Oni, Koropokguru, Hanuman</t>
   </si>
   <si>
@@ -3467,9 +3455,6 @@
     <t>That's a myth.</t>
   </si>
   <si>
-    <t>Succubus, Lilim</t>
-  </si>
-  <si>
     <t>Bicorn, Berith, Koropokguru, Anubis, Decarabia, Fuu-ki, Thor, Abaddon</t>
   </si>
   <si>
@@ -3509,9 +3494,6 @@
     <t>Agathion, Onmoraki, Obariyon</t>
   </si>
   <si>
-    <t>Agathion, Sudama</t>
-  </si>
-  <si>
     <t>Skadi, Rangda, Kali, Dakini</t>
   </si>
   <si>
@@ -3621,6 +3603,27 @@
   </si>
   <si>
     <t>Ippon-Datara, Bicorn, Berith, Oni, Anubis, Belphegor, Hanuman, Kumbhanda, Koropokguru</t>
+  </si>
+  <si>
+    <t>Succubus, Angel, Mandrake, Pixie</t>
+  </si>
+  <si>
+    <t>Mandrake, Angel, Lilim, Pixie</t>
+  </si>
+  <si>
+    <t>Berith, Koropokguru, Oni, Belphegor, Kumbhanda, Hanuman, Decarabia</t>
+  </si>
+  <si>
+    <t>Mandrake, Succubus, Angel, Lilim, Pixie</t>
+  </si>
+  <si>
+    <t>Agathion, Sudama, Obariyon</t>
+  </si>
+  <si>
+    <t>Mandrake, Succubus, Lilim, Pixie</t>
+  </si>
+  <si>
+    <t>Succubus, Lilim, Mandrake</t>
   </si>
 </sst>
 </file>
@@ -4462,8 +4465,8 @@
   <dimension ref="A1:S260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L133" sqref="L133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4599,32 +4602,32 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>1154</v>
+        <v>1149</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D3" s="5" t="str">
         <f t="shared" si="0"/>
         <v>after confronting me like this are you that kind of human too</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>1038</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1039</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>16</v>
@@ -4657,7 +4660,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>18</v>
@@ -4715,7 +4718,7 @@
     <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>23</v>
@@ -4773,7 +4776,7 @@
     <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>27</v>
@@ -4831,7 +4834,7 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>31</v>
@@ -4889,7 +4892,7 @@
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>35</v>
@@ -4947,7 +4950,7 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>39</v>
@@ -5005,7 +5008,7 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>1159</v>
+        <v>1195</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
@@ -5035,8 +5038,8 @@
       <c r="K10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>12</v>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>16</v>
@@ -5063,7 +5066,7 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>46</v>
@@ -5105,8 +5108,8 @@
       <c r="O11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P11" s="5" t="s">
-        <v>12</v>
+      <c r="P11" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>12</v>
@@ -5121,7 +5124,7 @@
     <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>50</v>
@@ -5237,7 +5240,7 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>58</v>
@@ -5295,7 +5298,7 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>62</v>
@@ -5353,7 +5356,7 @@
     <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>66</v>
@@ -5411,7 +5414,7 @@
     <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>70</v>
@@ -5469,7 +5472,7 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>74</v>
@@ -5527,7 +5530,7 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>78</v>
@@ -5653,7 +5656,7 @@
         <v>could this be what you humans call a proposal</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>12</v>
@@ -5668,7 +5671,7 @@
         <v>12</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>12</v>
@@ -5683,7 +5686,7 @@
         <v>12</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>12</v>
@@ -5701,10 +5704,10 @@
     <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D22" s="5" t="str">
         <f t="shared" si="0"/>
@@ -5759,7 +5762,7 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>89</v>
@@ -5817,7 +5820,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>93</v>
@@ -5875,7 +5878,7 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>97</v>
@@ -5896,8 +5899,8 @@
       <c r="H25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>13</v>
+      <c r="I25" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>99</v>
@@ -5933,7 +5936,7 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>101</v>
@@ -5991,7 +5994,7 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>105</v>
@@ -6049,7 +6052,7 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>109</v>
@@ -6165,7 +6168,7 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>117</v>
@@ -6189,7 +6192,7 @@
       <c r="I30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="2" t="s">
         <v>119</v>
       </c>
       <c r="K30" s="5" t="s">
@@ -6198,8 +6201,8 @@
       <c r="L30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M30" s="5" t="s">
-        <v>12</v>
+      <c r="M30" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>12</v>
@@ -6225,7 +6228,7 @@
         <v>862</v>
       </c>
       <c r="C31" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
       <c r="D31" s="5" t="str">
         <f t="shared" si="0"/>
@@ -6247,7 +6250,7 @@
         <v>12</v>
       </c>
       <c r="J31" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
       <c r="K31" t="s">
         <v>12</v>
@@ -6262,7 +6265,7 @@
         <v>12</v>
       </c>
       <c r="O31" t="s">
-        <v>1182</v>
+        <v>1176</v>
       </c>
       <c r="P31" t="s">
         <v>12</v>
@@ -6280,7 +6283,7 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>122</v>
@@ -6338,7 +6341,7 @@
     <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>126</v>
@@ -6396,7 +6399,7 @@
     <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>130</v>
@@ -6454,7 +6457,7 @@
     <row r="35" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>134</v>
@@ -6512,7 +6515,7 @@
     <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>138</v>
@@ -6563,14 +6566,14 @@
       <c r="R36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S36" s="5" t="s">
-        <v>12</v>
+      <c r="S36" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>142</v>
@@ -6628,7 +6631,7 @@
     <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>146</v>
@@ -6686,7 +6689,7 @@
     <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>149</v>
@@ -6744,7 +6747,7 @@
     <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="s">
-        <v>1045</v>
+        <v>1192</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>850</v>
@@ -6762,8 +6765,8 @@
       <c r="G40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>12</v>
+      <c r="H40" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>13</v>
@@ -6802,7 +6805,7 @@
     <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>156</v>
@@ -6860,7 +6863,7 @@
     <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>160</v>
@@ -6920,7 +6923,7 @@
         <v>121</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>164</v>
@@ -6978,7 +6981,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>168</v>
@@ -7038,7 +7041,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>172</v>
@@ -7096,10 +7099,10 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D46" s="5" t="str">
         <f t="shared" si="0"/>
@@ -7144,8 +7147,8 @@
       <c r="Q46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R46" s="2" t="s">
-        <v>13</v>
+      <c r="R46" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>13</v>
@@ -7154,7 +7157,7 @@
     <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>178</v>
@@ -7270,7 +7273,7 @@
     <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>186</v>
@@ -7328,7 +7331,7 @@
     <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>190</v>
@@ -7388,7 +7391,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>917</v>
@@ -7446,7 +7449,7 @@
     <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>197</v>
@@ -7506,7 +7509,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>204</v>
@@ -7564,7 +7567,7 @@
     <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>201</v>
@@ -7622,7 +7625,7 @@
     <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>208</v>
@@ -7680,7 +7683,7 @@
     <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>887</v>
@@ -7738,7 +7741,7 @@
     <row r="57" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>211</v>
@@ -7798,7 +7801,7 @@
         <v>22</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>215</v>
@@ -7856,7 +7859,7 @@
     <row r="59" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>219</v>
@@ -7914,7 +7917,7 @@
     <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="s">
-        <v>1173</v>
+        <v>1167</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>223</v>
@@ -7974,7 +7977,7 @@
         <v>121</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>906</v>
@@ -8032,7 +8035,7 @@
     <row r="62" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>227</v>
@@ -8148,7 +8151,7 @@
     <row r="64" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>867</v>
@@ -8206,7 +8209,7 @@
     <row r="65" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>231</v>
@@ -8263,17 +8266,17 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" t="s">
-        <v>1155</v>
+        <v>1150</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D66" s="5" t="str">
         <f t="shared" ref="D66:D129" si="1">LOWER(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C66,"?",""),"'",""),"-"," "),":",""),";"," "),"!"," "),","," "),"."," ")))</f>
         <v>i guess women are really more social these days finding so many fun things to do outside</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>13</v>
@@ -8288,7 +8291,7 @@
         <v>14</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="K66" t="s">
         <v>12</v>
@@ -8321,7 +8324,7 @@
     <row r="67" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5"/>
       <c r="B67" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>235</v>
@@ -8379,7 +8382,7 @@
     <row r="68" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5"/>
       <c r="B68" s="7" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>239</v>
@@ -8495,7 +8498,7 @@
     <row r="70" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="s">
-        <v>1176</v>
+        <v>1170</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>247</v>
@@ -8553,7 +8556,7 @@
     <row r="71" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>251</v>
@@ -8611,7 +8614,7 @@
     <row r="72" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>255</v>
@@ -8669,7 +8672,7 @@
     <row r="73" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>259</v>
@@ -8727,7 +8730,7 @@
     <row r="74" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5"/>
       <c r="B74" s="10" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>263</v>
@@ -8785,7 +8788,7 @@
     <row r="75" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>267</v>
@@ -8843,7 +8846,7 @@
     <row r="76" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>270</v>
@@ -8901,7 +8904,7 @@
     <row r="77" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>273</v>
@@ -8961,14 +8964,14 @@
         <v>875</v>
       </c>
       <c r="C78" t="s">
-        <v>1191</v>
+        <v>1185</v>
       </c>
       <c r="D78" s="5" t="str">
         <f t="shared" si="1"/>
         <v>i was going to catch a great buy live a life of celebrity whered it all go wrong</v>
       </c>
       <c r="E78" t="s">
-        <v>1193</v>
+        <v>1187</v>
       </c>
       <c r="F78" t="s">
         <v>12</v>
@@ -8983,7 +8986,7 @@
         <v>12</v>
       </c>
       <c r="J78" t="s">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="K78" t="s">
         <v>12</v>
@@ -8998,7 +9001,7 @@
         <v>12</v>
       </c>
       <c r="O78" t="s">
-        <v>1195</v>
+        <v>1189</v>
       </c>
       <c r="P78" t="s">
         <v>12</v>
@@ -9016,7 +9019,7 @@
     <row r="79" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>277</v>
@@ -9134,7 +9137,7 @@
         <v>121</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>289</v>
@@ -9192,7 +9195,7 @@
     <row r="82" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5"/>
       <c r="B82" s="5" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>285</v>
@@ -9250,7 +9253,7 @@
     <row r="83" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5"/>
       <c r="B83" s="5" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>293</v>
@@ -9308,7 +9311,7 @@
     <row r="84" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5"/>
       <c r="B84" s="5" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>297</v>
@@ -9366,7 +9369,7 @@
     <row r="85" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5"/>
       <c r="B85" s="5" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>301</v>
@@ -9424,7 +9427,7 @@
     <row r="86" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="5"/>
       <c r="B86" s="5" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>305</v>
@@ -9482,7 +9485,7 @@
     <row r="87" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5"/>
       <c r="B87" s="5" t="s">
-        <v>1098</v>
+        <v>1191</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>309</v>
@@ -9521,7 +9524,7 @@
       <c r="N87" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O87" s="5" t="s">
+      <c r="O87" s="2" t="s">
         <v>312</v>
       </c>
       <c r="P87" s="5" t="s">
@@ -9530,8 +9533,8 @@
       <c r="Q87" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R87" s="5" t="s">
-        <v>12</v>
+      <c r="R87" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="S87" s="5" t="s">
         <v>12</v>
@@ -9540,7 +9543,7 @@
     <row r="88" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
-        <v>1196</v>
+        <v>1190</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>313</v>
@@ -9598,7 +9601,7 @@
     <row r="89" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5"/>
       <c r="B89" s="5" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>317</v>
@@ -9656,7 +9659,7 @@
     <row r="90" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>321</v>
@@ -9714,7 +9717,7 @@
     <row r="91" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>325</v>
@@ -9772,7 +9775,7 @@
     <row r="92" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="5"/>
       <c r="B92" s="5" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>329</v>
@@ -9830,7 +9833,7 @@
     <row r="93" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="5"/>
       <c r="B93" s="5" t="s">
-        <v>1145</v>
+        <v>1197</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>333</v>
@@ -9851,8 +9854,8 @@
       <c r="H93" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I93" s="5" t="s">
-        <v>12</v>
+      <c r="I93" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>335</v>
@@ -9887,17 +9890,17 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="D94" s="5" t="str">
         <f t="shared" si="1"/>
         <v>ill let you kill me but first i want you to do something fun for me before that</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
@@ -9912,7 +9915,7 @@
         <v>12</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="K94" t="s">
         <v>12</v>
@@ -9927,7 +9930,7 @@
         <v>12</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="P94" s="2" t="s">
         <v>14</v>
@@ -10003,7 +10006,7 @@
     <row r="96" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="5"/>
       <c r="B96" s="5" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>341</v>
@@ -10061,7 +10064,7 @@
     <row r="97" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5"/>
       <c r="B97" s="5" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>345</v>
@@ -10119,7 +10122,7 @@
     <row r="98" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="5"/>
       <c r="B98" s="5" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>857</v>
@@ -10237,7 +10240,7 @@
         <v>22</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>354</v>
@@ -10295,7 +10298,7 @@
     <row r="101" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="5"/>
       <c r="B101" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>357</v>
@@ -10352,17 +10355,17 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B102" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="D102" s="5" t="str">
         <f t="shared" si="1"/>
         <v>im so sleepy ho i just want you to leave me alone</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>13</v>
@@ -10377,7 +10380,7 @@
         <v>12</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="K102" t="s">
         <v>12</v>
@@ -10392,7 +10395,7 @@
         <v>12</v>
       </c>
       <c r="O102" s="2" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="P102" t="s">
         <v>12</v>
@@ -10410,7 +10413,7 @@
     <row r="103" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="5"/>
       <c r="B103" s="5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>360</v>
@@ -10468,7 +10471,7 @@
     <row r="104" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="5"/>
       <c r="B104" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>364</v>
@@ -10526,7 +10529,7 @@
     <row r="105" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="5"/>
       <c r="B105" s="5" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>368</v>
@@ -10584,7 +10587,7 @@
     <row r="106" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="5"/>
       <c r="B106" s="5" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>371</v>
@@ -10642,7 +10645,7 @@
     <row r="107" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="5"/>
       <c r="B107" s="5" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>375</v>
@@ -10758,7 +10761,7 @@
     <row r="109" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="5"/>
       <c r="B109" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>383</v>
@@ -10816,7 +10819,7 @@
     <row r="110" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="5"/>
       <c r="B110" s="5" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>385</v>
@@ -10873,17 +10876,17 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" t="s">
-        <v>1184</v>
+        <v>1178</v>
       </c>
       <c r="C111" t="s">
-        <v>1192</v>
+        <v>1186</v>
       </c>
       <c r="D111" s="5" t="str">
         <f t="shared" si="1"/>
         <v>is it ok if i get mad right now</v>
       </c>
       <c r="E111" t="s">
-        <v>1188</v>
+        <v>1182</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
@@ -10913,7 +10916,7 @@
         <v>12</v>
       </c>
       <c r="O111" t="s">
-        <v>1189</v>
+        <v>1183</v>
       </c>
       <c r="P111" t="s">
         <v>12</v>
@@ -10931,7 +10934,7 @@
     <row r="112" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="5"/>
       <c r="B112" s="5" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>388</v>
@@ -10998,14 +11001,14 @@
         <f t="shared" si="1"/>
         <v>is there a reason why i just cant beat you</v>
       </c>
-      <c r="E113" s="5" t="s">
+      <c r="E113" s="2" t="s">
         <v>393</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G113" s="5" t="s">
-        <v>12</v>
+      <c r="G113" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>12</v>
@@ -11047,7 +11050,7 @@
     <row r="114" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="5"/>
       <c r="B114" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>396</v>
@@ -11105,7 +11108,7 @@
     <row r="115" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="5"/>
       <c r="B115" s="5" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>400</v>
@@ -11221,7 +11224,7 @@
     <row r="117" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="5"/>
       <c r="B117" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>405</v>
@@ -11279,7 +11282,7 @@
     <row r="118" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="5"/>
       <c r="B118" s="5" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>409</v>
@@ -11337,7 +11340,7 @@
     <row r="119" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="5"/>
       <c r="B119" s="5" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>413</v>
@@ -11395,7 +11398,7 @@
     <row r="120" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="5"/>
       <c r="B120" s="5" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>876</v>
@@ -11453,7 +11456,7 @@
     <row r="121" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="5"/>
       <c r="B121" s="5" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>420</v>
@@ -11511,7 +11514,7 @@
     <row r="122" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="5"/>
       <c r="B122" s="5" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>424</v>
@@ -11553,7 +11556,7 @@
       <c r="O122" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="P122" s="5" t="s">
+      <c r="P122" s="2" t="s">
         <v>16</v>
       </c>
       <c r="Q122" s="5" t="s">
@@ -11569,7 +11572,7 @@
     <row r="123" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="5"/>
       <c r="B123" s="5" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>428</v>
@@ -11627,7 +11630,7 @@
     <row r="124" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="5"/>
       <c r="B124" s="5" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>432</v>
@@ -11743,7 +11746,7 @@
     <row r="126" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="5"/>
       <c r="B126" s="5" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>439</v>
@@ -11801,7 +11804,7 @@
     <row r="127" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="5"/>
       <c r="B127" s="5" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>442</v>
@@ -11859,7 +11862,7 @@
     <row r="128" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="5"/>
       <c r="B128" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>445</v>
@@ -11917,7 +11920,7 @@
     <row r="129" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="5"/>
       <c r="B129" s="5" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>453</v>
@@ -11975,7 +11978,7 @@
     <row r="130" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="5"/>
       <c r="B130" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>457</v>
@@ -12033,7 +12036,7 @@
     <row r="131" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="5"/>
       <c r="B131" s="5" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>449</v>
@@ -12091,7 +12094,7 @@
     <row r="132" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="5"/>
       <c r="B132" s="5" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>461</v>
@@ -12149,7 +12152,7 @@
     <row r="133" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="5"/>
       <c r="B133" s="5" t="s">
-        <v>1177</v>
+        <v>1171</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>465</v>
@@ -12179,7 +12182,7 @@
       <c r="K133" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L133" s="5" t="s">
+      <c r="L133" s="2" t="s">
         <v>13</v>
       </c>
       <c r="M133" s="2" t="s">
@@ -12207,7 +12210,7 @@
     <row r="134" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="5"/>
       <c r="B134" s="5" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>469</v>
@@ -12265,7 +12268,7 @@
     <row r="135" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="5"/>
       <c r="B135" s="5" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>473</v>
@@ -12323,7 +12326,7 @@
     <row r="136" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="5"/>
       <c r="B136" s="5" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>477</v>
@@ -12381,7 +12384,7 @@
     <row r="137" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="5"/>
       <c r="B137" s="5" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>481</v>
@@ -12439,7 +12442,7 @@
     <row r="138" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="5"/>
       <c r="B138" s="5" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>485</v>
@@ -12497,7 +12500,7 @@
     <row r="139" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="5"/>
       <c r="B139" s="5" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>489</v>
@@ -12555,7 +12558,7 @@
     <row r="140" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="5"/>
       <c r="B140" s="5" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>493</v>
@@ -12613,7 +12616,7 @@
     <row r="141" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="5"/>
       <c r="B141" s="5" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>497</v>
@@ -12671,7 +12674,7 @@
     <row r="142" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="5"/>
       <c r="B142" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>501</v>
@@ -12786,47 +12789,47 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" t="s">
-        <v>1160</v>
+        <v>1154</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D144" s="5" t="str">
         <f t="shared" si="2"/>
         <v>now people dont even know who lives next door to them shouldnt we know our neighbors better</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H144" t="s">
+        <v>12</v>
+      </c>
+      <c r="I144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J144" t="s">
+        <v>1088</v>
+      </c>
+      <c r="K144" t="s">
+        <v>12</v>
+      </c>
+      <c r="L144" t="s">
+        <v>12</v>
+      </c>
+      <c r="M144" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N144" t="s">
+        <v>12</v>
+      </c>
+      <c r="O144" t="s">
         <v>1089</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H144" t="s">
-        <v>12</v>
-      </c>
-      <c r="I144" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J144" t="s">
-        <v>1090</v>
-      </c>
-      <c r="K144" t="s">
-        <v>12</v>
-      </c>
-      <c r="L144" t="s">
-        <v>12</v>
-      </c>
-      <c r="M144" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N144" t="s">
-        <v>12</v>
-      </c>
-      <c r="O144" t="s">
-        <v>1091</v>
       </c>
       <c r="P144" t="s">
         <v>12</v>
@@ -12844,7 +12847,7 @@
     <row r="145" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="5"/>
       <c r="B145" s="5" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>506</v>
@@ -12902,7 +12905,7 @@
     <row r="146" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="5"/>
       <c r="B146" s="5" t="s">
-        <v>996</v>
+        <v>1194</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>507</v>
@@ -12950,8 +12953,8 @@
       <c r="Q146" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R146" s="5" t="s">
-        <v>12</v>
+      <c r="R146" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="S146" s="4" t="s">
         <v>13</v>
@@ -13018,7 +13021,7 @@
     <row r="148" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="5"/>
       <c r="B148" s="5" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>511</v>
@@ -13076,7 +13079,7 @@
     <row r="149" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="5"/>
       <c r="B149" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>514</v>
@@ -13134,7 +13137,7 @@
     <row r="150" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="5"/>
       <c r="B150" s="5" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>518</v>
@@ -13192,7 +13195,7 @@
     <row r="151" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="5"/>
       <c r="B151" s="5" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>522</v>
@@ -13250,7 +13253,7 @@
     <row r="152" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="5"/>
       <c r="B152" s="7" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>526</v>
@@ -13308,7 +13311,7 @@
     <row r="153" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="5"/>
       <c r="B153" s="7" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>529</v>
@@ -13366,7 +13369,7 @@
     <row r="154" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="5"/>
       <c r="B154" s="5" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>533</v>
@@ -13424,7 +13427,7 @@
     <row r="155" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="5"/>
       <c r="B155" s="5" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>537</v>
@@ -13482,7 +13485,7 @@
     <row r="156" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="5"/>
       <c r="B156" s="5" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>541</v>
@@ -13542,44 +13545,44 @@
         <v>891</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D157" s="5" t="str">
         <f t="shared" si="2"/>
         <v>some old people refuse to make use of special seats reserved for the elderly what do you think of that</v>
       </c>
       <c r="E157" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F157" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" t="s">
+        <v>12</v>
+      </c>
+      <c r="H157" t="s">
+        <v>12</v>
+      </c>
+      <c r="I157" t="s">
+        <v>12</v>
+      </c>
+      <c r="J157" s="2" t="s">
         <v>1032</v>
       </c>
-      <c r="F157" t="s">
-        <v>12</v>
-      </c>
-      <c r="G157" t="s">
-        <v>12</v>
-      </c>
-      <c r="H157" t="s">
-        <v>12</v>
-      </c>
-      <c r="I157" t="s">
-        <v>12</v>
-      </c>
-      <c r="J157" s="2" t="s">
+      <c r="K157" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L157" t="s">
+        <v>12</v>
+      </c>
+      <c r="M157" t="s">
+        <v>12</v>
+      </c>
+      <c r="N157" t="s">
+        <v>12</v>
+      </c>
+      <c r="O157" s="2" t="s">
         <v>1033</v>
-      </c>
-      <c r="K157" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L157" t="s">
-        <v>12</v>
-      </c>
-      <c r="M157" t="s">
-        <v>12</v>
-      </c>
-      <c r="N157" t="s">
-        <v>12</v>
-      </c>
-      <c r="O157" s="2" t="s">
-        <v>1034</v>
       </c>
       <c r="P157" t="s">
         <v>12</v>
@@ -13597,7 +13600,7 @@
     <row r="158" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="5"/>
       <c r="B158" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>545</v>
@@ -13655,7 +13658,7 @@
     <row r="159" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="5"/>
       <c r="B159" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>549</v>
@@ -13713,7 +13716,7 @@
     <row r="160" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="5"/>
       <c r="B160" s="5" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>553</v>
@@ -13771,7 +13774,7 @@
     <row r="161" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="5"/>
       <c r="B161" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>556</v>
@@ -13829,7 +13832,7 @@
     <row r="162" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="5"/>
       <c r="B162" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>559</v>
@@ -13889,14 +13892,14 @@
         <v>862</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="D163" s="5" t="str">
         <f t="shared" si="2"/>
         <v>that is to say we are brothers there is no reason for us to fight</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="F163" t="s">
         <v>12</v>
@@ -13911,7 +13914,7 @@
         <v>12</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
       <c r="K163" t="s">
         <v>12</v>
@@ -13926,7 +13929,7 @@
         <v>12</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="P163" t="s">
         <v>12</v>
@@ -13944,7 +13947,7 @@
     <row r="164" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="5"/>
       <c r="B164" s="5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>563</v>
@@ -14060,7 +14063,7 @@
     <row r="166" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="5"/>
       <c r="B166" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>863</v>
@@ -14176,10 +14179,10 @@
     <row r="168" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="5"/>
       <c r="B168" s="5" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D168" s="5" t="str">
         <f t="shared" si="2"/>
@@ -14233,47 +14236,47 @@
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B169" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D169" s="5" t="str">
         <f t="shared" si="2"/>
         <v>the least i can do is extend this small mercy confess the calamity that you can bear</v>
       </c>
       <c r="E169" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G169" t="s">
+        <v>12</v>
+      </c>
+      <c r="H169" t="s">
+        <v>12</v>
+      </c>
+      <c r="I169" t="s">
+        <v>12</v>
+      </c>
+      <c r="J169" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="F169" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G169" t="s">
-        <v>12</v>
-      </c>
-      <c r="H169" t="s">
-        <v>12</v>
-      </c>
-      <c r="I169" t="s">
-        <v>12</v>
-      </c>
-      <c r="J169" s="2" t="s">
+      <c r="K169" t="s">
+        <v>12</v>
+      </c>
+      <c r="L169" s="12" t="s">
+        <v>1027</v>
+      </c>
+      <c r="M169" t="s">
+        <v>12</v>
+      </c>
+      <c r="N169" t="s">
+        <v>12</v>
+      </c>
+      <c r="O169" s="2" t="s">
         <v>939</v>
-      </c>
-      <c r="K169" t="s">
-        <v>12</v>
-      </c>
-      <c r="L169" s="12" t="s">
-        <v>1028</v>
-      </c>
-      <c r="M169" t="s">
-        <v>12</v>
-      </c>
-      <c r="N169" t="s">
-        <v>12</v>
-      </c>
-      <c r="O169" s="2" t="s">
-        <v>940</v>
       </c>
       <c r="P169" t="s">
         <v>12</v>
@@ -14291,7 +14294,7 @@
     <row r="170" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="5"/>
       <c r="B170" s="5" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>578</v>
@@ -14349,10 +14352,10 @@
     <row r="171" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="5"/>
       <c r="B171" s="5" t="s">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
       <c r="D171" s="5" t="str">
         <f t="shared" si="2"/>
@@ -14407,7 +14410,7 @@
     <row r="172" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="5"/>
       <c r="B172" s="5" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>585</v>
@@ -14465,10 +14468,10 @@
     <row r="173" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="5"/>
       <c r="B173" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D173" s="5" t="str">
         <f t="shared" si="2"/>
@@ -14523,7 +14526,7 @@
     <row r="174" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="5"/>
       <c r="B174" s="5" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>590</v>
@@ -14641,7 +14644,7 @@
         <v>22</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>597</v>
@@ -14699,7 +14702,7 @@
     <row r="177" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="5"/>
       <c r="B177" s="5" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>601</v>
@@ -14756,32 +14759,32 @@
     </row>
     <row r="178" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D178" s="5" t="str">
         <f t="shared" si="2"/>
         <v>to tell you the hee truth this is all an act ho what do you think im really like ho</v>
       </c>
       <c r="E178" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" t="s">
+        <v>12</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I178" t="s">
+        <v>12</v>
+      </c>
+      <c r="J178" s="2" t="s">
         <v>1020</v>
-      </c>
-      <c r="F178" t="s">
-        <v>12</v>
-      </c>
-      <c r="G178" t="s">
-        <v>12</v>
-      </c>
-      <c r="H178" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I178" t="s">
-        <v>12</v>
-      </c>
-      <c r="J178" s="2" t="s">
-        <v>1021</v>
       </c>
       <c r="K178" t="s">
         <v>12</v>
@@ -14814,7 +14817,7 @@
     <row r="179" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="5"/>
       <c r="B179" s="5" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>894</v>
@@ -14932,7 +14935,7 @@
     <row r="181" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="5"/>
       <c r="B181" s="5" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>609</v>
@@ -14990,7 +14993,7 @@
     <row r="182" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="5"/>
       <c r="B182" s="5" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>613</v>
@@ -15048,7 +15051,7 @@
     <row r="183" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="5"/>
       <c r="B183" s="5" t="s">
-        <v>1157</v>
+        <v>1152</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>616</v>
@@ -15106,7 +15109,7 @@
     <row r="184" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="5"/>
       <c r="B184" s="5" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>623</v>
@@ -15166,7 +15169,7 @@
         <v>121</v>
       </c>
       <c r="B185" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>627</v>
@@ -15224,7 +15227,7 @@
     <row r="186" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="5"/>
       <c r="B186" s="5" t="s">
-        <v>1097</v>
+        <v>1196</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>851</v>
@@ -15248,7 +15251,7 @@
       <c r="I186" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J186" s="5" t="s">
+      <c r="J186" s="2" t="s">
         <v>621</v>
       </c>
       <c r="K186" s="5" t="s">
@@ -15257,8 +15260,8 @@
       <c r="L186" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M186" s="5" t="s">
-        <v>12</v>
+      <c r="M186" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="N186" s="5" t="s">
         <v>12</v>
@@ -15281,10 +15284,10 @@
     </row>
     <row r="187" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D187" s="5" t="str">
         <f t="shared" si="2"/>
@@ -15339,7 +15342,7 @@
     <row r="188" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="5"/>
       <c r="B188" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>635</v>
@@ -15397,7 +15400,7 @@
     <row r="189" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="5"/>
       <c r="B189" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>639</v>
@@ -15455,7 +15458,7 @@
     <row r="190" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="5"/>
       <c r="B190" s="5" t="s">
-        <v>1153</v>
+        <v>1148</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>652</v>
@@ -15513,7 +15516,7 @@
     <row r="191" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="5"/>
       <c r="B191" s="5" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="C191" s="6" t="s">
         <v>643</v>
@@ -15629,7 +15632,7 @@
     <row r="193" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="5"/>
       <c r="B193" s="5" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>650</v>
@@ -15687,7 +15690,7 @@
     <row r="194" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="5"/>
       <c r="B194" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>884</v>
@@ -15727,7 +15730,7 @@
         <v>12</v>
       </c>
       <c r="O194" s="2" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="P194" s="5" t="s">
         <v>12</v>
@@ -15745,7 +15748,7 @@
     <row r="195" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="5"/>
       <c r="B195" s="5" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>656</v>
@@ -15803,7 +15806,7 @@
     <row r="196" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="5"/>
       <c r="B196" s="7" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>659</v>
@@ -15863,32 +15866,32 @@
         <v>121</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D197" s="5" t="str">
         <f t="shared" si="3"/>
         <v>what kind of place do you want to live in</v>
       </c>
       <c r="E197" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="F197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J197" s="2" t="s">
         <v>932</v>
-      </c>
-      <c r="F197" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G197" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H197" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I197" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J197" s="2" t="s">
-        <v>933</v>
       </c>
       <c r="K197" s="5" t="s">
         <v>12</v>
@@ -15921,7 +15924,7 @@
     <row r="198" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="5"/>
       <c r="B198" s="7" t="s">
-        <v>923</v>
+        <v>1193</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>663</v>
@@ -15948,8 +15951,8 @@
       <c r="J198" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="K198" s="5" t="s">
-        <v>12</v>
+      <c r="K198" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="L198" s="5" t="s">
         <v>16</v>
@@ -15979,7 +15982,7 @@
     <row r="199" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="5"/>
       <c r="B199" s="5" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>667</v>
@@ -16037,7 +16040,7 @@
     <row r="200" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="5"/>
       <c r="B200" s="5" t="s">
-        <v>1174</v>
+        <v>1168</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>671</v>
@@ -16047,7 +16050,7 @@
         <v>what should i wear</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>1175</v>
+        <v>1169</v>
       </c>
       <c r="F200" s="5" t="s">
         <v>12</v>
@@ -16095,7 +16098,7 @@
     <row r="201" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="5"/>
       <c r="B201" s="5" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>674</v>
@@ -16153,7 +16156,7 @@
     <row r="202" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="5"/>
       <c r="B202" s="5" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>678</v>
@@ -16211,7 +16214,7 @@
     <row r="203" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="5"/>
       <c r="B203" s="5" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>682</v>
@@ -16269,7 +16272,7 @@
     <row r="204" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="5"/>
       <c r="B204" s="5" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C204" s="6" t="s">
         <v>686</v>
@@ -16327,7 +16330,7 @@
     <row r="205" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="5"/>
       <c r="B205" s="5" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>690</v>
@@ -16385,7 +16388,7 @@
     <row r="206" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="5"/>
       <c r="B206" s="5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>694</v>
@@ -16443,7 +16446,7 @@
     <row r="207" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="5"/>
       <c r="B207" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>698</v>
@@ -16500,17 +16503,17 @@
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="D208" s="5" t="str">
         <f t="shared" si="3"/>
         <v>when it came right down to it you couldnt do anything to me</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>1185</v>
+        <v>1179</v>
       </c>
       <c r="F208" t="s">
         <v>12</v>
@@ -16525,7 +16528,7 @@
         <v>12</v>
       </c>
       <c r="J208" s="2" t="s">
-        <v>1186</v>
+        <v>1180</v>
       </c>
       <c r="K208" t="s">
         <v>12</v>
@@ -16540,7 +16543,7 @@
         <v>12</v>
       </c>
       <c r="O208" s="2" t="s">
-        <v>1187</v>
+        <v>1181</v>
       </c>
       <c r="P208" t="s">
         <v>12</v>
@@ -16558,7 +16561,7 @@
     <row r="209" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="5"/>
       <c r="B209" s="5" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>702</v>
@@ -16616,7 +16619,7 @@
     <row r="210" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="5"/>
       <c r="B210" s="5" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>706</v>
@@ -16647,7 +16650,7 @@
         <v>12</v>
       </c>
       <c r="L210" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M210" s="5" t="s">
         <v>12</v>
@@ -16674,7 +16677,7 @@
     <row r="211" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="5"/>
       <c r="B211" s="5" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>710</v>
@@ -16732,7 +16735,7 @@
     <row r="212" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="5"/>
       <c r="B212" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>631</v>
@@ -16790,7 +16793,7 @@
     <row r="213" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="5"/>
       <c r="B213" s="5" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>714</v>
@@ -16850,7 +16853,7 @@
         <v>912</v>
       </c>
       <c r="C214" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="D214" s="5" t="str">
         <f t="shared" si="3"/>
@@ -16902,7 +16905,7 @@
     <row r="215" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="5"/>
       <c r="B215" s="5" t="s">
-        <v>1161</v>
+        <v>1155</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>902</v>
@@ -16960,7 +16963,7 @@
     <row r="216" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="5"/>
       <c r="B216" s="5" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>852</v>
@@ -17018,7 +17021,7 @@
     <row r="217" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5"/>
       <c r="B217" s="5" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>720</v>
@@ -17076,7 +17079,7 @@
     <row r="218" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="5"/>
       <c r="B218" s="5" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>724</v>
@@ -17134,7 +17137,7 @@
     <row r="219" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="5"/>
       <c r="B219" s="5" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>728</v>
@@ -17192,7 +17195,7 @@
     <row r="220" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="5"/>
       <c r="B220" s="5" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>732</v>
@@ -17250,7 +17253,7 @@
     <row r="221" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="5"/>
       <c r="B221" s="5" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>736</v>
@@ -17308,7 +17311,7 @@
     <row r="222" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="5"/>
       <c r="B222" s="5" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>740</v>
@@ -17366,7 +17369,7 @@
     <row r="223" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="5"/>
       <c r="B223" s="5" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>744</v>
@@ -17426,7 +17429,7 @@
         <v>22</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>911</v>
@@ -17483,17 +17486,17 @@
     </row>
     <row r="225" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D225" s="5" t="str">
         <f t="shared" si="3"/>
         <v>would you be willing to spend time and money to see people you havent contacted for years</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F225" t="s">
         <v>12</v>
@@ -17508,7 +17511,7 @@
         <v>12</v>
       </c>
       <c r="J225" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="K225" t="s">
         <v>12</v>
@@ -17523,7 +17526,7 @@
         <v>12</v>
       </c>
       <c r="O225" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="P225" t="s">
         <v>12</v>
@@ -17541,7 +17544,7 @@
     <row r="226" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="5"/>
       <c r="B226" s="5" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C226" s="6" t="s">
         <v>751</v>
@@ -17601,7 +17604,7 @@
         <v>22</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>755</v>
@@ -17659,7 +17662,7 @@
     <row r="228" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="5"/>
       <c r="B228" s="5" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C228" s="6" t="s">
         <v>759</v>
@@ -17717,7 +17720,7 @@
     <row r="229" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="5"/>
       <c r="B229" s="5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>763</v>
@@ -17775,7 +17778,7 @@
     <row r="230" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="5"/>
       <c r="B230" s="5" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>767</v>
@@ -17833,7 +17836,7 @@
     <row r="231" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="5"/>
       <c r="B231" s="5" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>770</v>
@@ -17949,7 +17952,7 @@
     <row r="233" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="5"/>
       <c r="B233" s="5" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>774</v>
@@ -18007,7 +18010,7 @@
     <row r="234" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="5"/>
       <c r="B234" s="5" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C234" s="6" t="s">
         <v>777</v>
@@ -18065,7 +18068,7 @@
     <row r="235" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="5"/>
       <c r="B235" s="5" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C235" s="6" t="s">
         <v>781</v>
@@ -18123,7 +18126,7 @@
     <row r="236" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="5"/>
       <c r="B236" s="5" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C236" s="6" t="s">
         <v>785</v>
@@ -18183,7 +18186,7 @@
         <v>862</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="D237" s="5" t="str">
         <f t="shared" si="3"/>
@@ -18205,7 +18208,7 @@
         <v>12</v>
       </c>
       <c r="J237" s="2" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="K237" t="s">
         <v>12</v>
@@ -18238,7 +18241,7 @@
     <row r="238" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="5"/>
       <c r="B238" s="5" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C238" s="6" t="s">
         <v>789</v>
@@ -18296,10 +18299,10 @@
     <row r="239" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="5"/>
       <c r="B239" s="5" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="D239" s="5" t="str">
         <f t="shared" si="3"/>
@@ -18354,7 +18357,7 @@
     <row r="240" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="5"/>
       <c r="B240" s="5" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C240" s="6" t="s">
         <v>796</v>
@@ -18412,7 +18415,7 @@
     <row r="241" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="5"/>
       <c r="B241" s="5" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C241" s="6" t="s">
         <v>799</v>
@@ -18470,7 +18473,7 @@
     <row r="242" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="5"/>
       <c r="B242" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>802</v>
@@ -18528,7 +18531,7 @@
     <row r="243" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="5"/>
       <c r="B243" s="5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C243" s="6" t="s">
         <v>806</v>
@@ -18644,7 +18647,7 @@
     <row r="245" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="5"/>
       <c r="B245" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C245" s="6" t="s">
         <v>814</v>
@@ -18702,7 +18705,7 @@
     <row r="246" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="5"/>
       <c r="B246" s="5" t="s">
-        <v>1160</v>
+        <v>1154</v>
       </c>
       <c r="C246" s="6" t="s">
         <v>898</v>
@@ -18717,8 +18720,8 @@
       <c r="F246" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G246" s="5" t="s">
-        <v>12</v>
+      <c r="G246" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H246" s="5" t="s">
         <v>12</v>
@@ -18760,7 +18763,7 @@
     <row r="247" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="5"/>
       <c r="B247" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>817</v>
@@ -18818,7 +18821,7 @@
     <row r="248" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="5"/>
       <c r="B248" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C248" s="6" t="s">
         <v>820</v>
@@ -18875,10 +18878,10 @@
     </row>
     <row r="249" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B249" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D249" s="5" t="str">
         <f t="shared" si="3"/>
@@ -18915,7 +18918,7 @@
         <v>12</v>
       </c>
       <c r="O249" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="P249" s="2" t="s">
         <v>16</v>
@@ -18932,7 +18935,7 @@
     </row>
     <row r="250" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C250" s="3" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="D250" s="5" t="str">
         <f t="shared" si="3"/>
@@ -18954,7 +18957,7 @@
         <v>12</v>
       </c>
       <c r="J250" s="2" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="K250" t="s">
         <v>12</v>
@@ -18969,7 +18972,7 @@
         <v>12</v>
       </c>
       <c r="O250" s="2" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="P250" t="s">
         <v>12</v>
@@ -18987,7 +18990,7 @@
     <row r="251" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="5"/>
       <c r="B251" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C251" s="6" t="s">
         <v>821</v>
@@ -19044,17 +19047,17 @@
     </row>
     <row r="252" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B252" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D252" s="5" t="str">
         <f t="shared" si="3"/>
         <v>youll have a bleak future if you spend too much time running around pretending to be a phantom thief</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F252" s="2" t="s">
         <v>13</v>
@@ -19084,7 +19087,7 @@
         <v>12</v>
       </c>
       <c r="O252" s="2" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="P252" t="s">
         <v>12</v>
@@ -19102,7 +19105,7 @@
     <row r="253" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="5"/>
       <c r="B253" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C253" s="6" t="s">
         <v>825</v>
@@ -19160,7 +19163,7 @@
     <row r="254" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="5"/>
       <c r="B254" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C254" s="6" t="s">
         <v>829</v>
@@ -19218,7 +19221,7 @@
     <row r="255" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="5"/>
       <c r="B255" s="5" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="C255" s="6" t="s">
         <v>853</v>
@@ -19276,7 +19279,7 @@
     <row r="256" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="5"/>
       <c r="B256" s="5" t="s">
-        <v>1169</v>
+        <v>1163</v>
       </c>
       <c r="C256" s="6" t="s">
         <v>832</v>
@@ -19334,7 +19337,7 @@
     <row r="257" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="5"/>
       <c r="B257" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C257" s="6" t="s">
         <v>835</v>
@@ -19392,7 +19395,7 @@
     <row r="258" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="5"/>
       <c r="B258" s="5" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C258" s="6" t="s">
         <v>839</v>
@@ -19450,7 +19453,7 @@
     <row r="259" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="5"/>
       <c r="B259" s="5" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C259" s="6" t="s">
         <v>842</v>
@@ -19508,7 +19511,7 @@
     <row r="260" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="5"/>
       <c r="B260" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C260" s="6" t="s">
         <v>846</v>

</xml_diff>

<commit_message>
Added 182 entries from form (3/09 15:42)
Plus 3 entries from Issue #16
</commit_message>
<xml_diff>
--- a/data/persona-5-questions.xlsx
+++ b/data/persona-5-questions.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joyce\Documents\GitHub\persona5-negotiation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087D91CF-A2BB-4747-95C2-8CE305BDCDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89495D93-8245-48C5-A716-4415A23C48C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2562" yWindow="2562" windowWidth="17436" windowHeight="8628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9690" yWindow="1056" windowWidth="13242" windowHeight="10614" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="1197">
   <si>
     <t>Flag</t>
   </si>
@@ -2939,9 +2929,6 @@
     <t>Dakini</t>
   </si>
   <si>
-    <t>Rangda, Dakini</t>
-  </si>
-  <si>
     <t>Kelpie, Slime, Unicorn, Mothman, Arahabaki, Thoth, Anzu, Orthrus, Shiki-Ouji, Makami, Inugami, Andras</t>
   </si>
   <si>
@@ -3474,9 +3461,6 @@
   </si>
   <si>
     <t>Skadi, Rangda, Kali, Dakini</t>
-  </si>
-  <si>
-    <t>Rangda, Kali, Dakini</t>
   </si>
   <si>
     <t>Naga, Oberon, Mithras, Mokoi, Barong</t>
@@ -4461,8 +4445,8 @@
   <dimension ref="A1:S260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4597,32 +4581,32 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>after confronting me like this are you that kind of human too</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>1031</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1032</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>16</v>
@@ -4825,7 +4809,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
@@ -4882,7 +4866,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>35</v>
@@ -4939,7 +4923,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>39</v>
@@ -4996,7 +4980,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>43</v>
@@ -5224,7 +5208,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>58</v>
@@ -5281,7 +5265,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>62</v>
@@ -5395,7 +5379,7 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>70</v>
@@ -5452,7 +5436,7 @@
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>74</v>
@@ -5509,7 +5493,7 @@
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>78</v>
@@ -5566,7 +5550,7 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>82</v>
@@ -5633,37 +5617,37 @@
         <v>could this be what you humans call a proposal</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>1131</v>
       </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>1132</v>
-      </c>
-      <c r="K21" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21" t="s">
-        <v>12</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>1133</v>
       </c>
       <c r="P21" t="s">
         <v>12</v>
@@ -5683,7 +5667,7 @@
         <v>922</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -5737,7 +5721,7 @@
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>89</v>
@@ -5794,7 +5778,7 @@
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>93</v>
@@ -5851,7 +5835,7 @@
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>97</v>
@@ -5908,7 +5892,7 @@
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>101</v>
@@ -5965,7 +5949,7 @@
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>105</v>
@@ -6196,7 +6180,7 @@
         <v>862</v>
       </c>
       <c r="C31" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -6218,7 +6202,7 @@
         <v>12</v>
       </c>
       <c r="J31" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="K31" t="s">
         <v>12</v>
@@ -6233,7 +6217,7 @@
         <v>12</v>
       </c>
       <c r="O31" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="P31" t="s">
         <v>12</v>
@@ -6250,7 +6234,7 @@
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>122</v>
@@ -6307,7 +6291,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>126</v>
@@ -6364,7 +6348,7 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>130</v>
@@ -6478,7 +6462,7 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>138</v>
@@ -6535,7 +6519,7 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>142</v>
@@ -6592,7 +6576,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>146</v>
@@ -6649,7 +6633,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>149</v>
@@ -6706,7 +6690,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>850</v>
@@ -6763,7 +6747,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>156</v>
@@ -6820,7 +6804,7 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>160</v>
@@ -6880,7 +6864,7 @@
         <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>164</v>
@@ -6937,7 +6921,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>168</v>
@@ -6997,7 +6981,7 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>172</v>
@@ -7057,7 +7041,7 @@
         <v>942</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -7111,7 +7095,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>178</v>
@@ -7282,7 +7266,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>190</v>
@@ -7342,7 +7326,7 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>916</v>
@@ -7399,7 +7383,7 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>197</v>
@@ -7459,7 +7443,7 @@
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>204</v>
@@ -7516,7 +7500,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>201</v>
@@ -7630,7 +7614,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>887</v>
@@ -7861,7 +7845,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>223</v>
@@ -7978,7 +7962,7 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>227</v>
@@ -8092,7 +8076,7 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>867</v>
@@ -8149,7 +8133,7 @@
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>231</v>
@@ -8206,32 +8190,32 @@
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D129" si="1">LOWER(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C66,"?",""),"'",""),"-"," "),":",""),";"," "),"!"," "),","," "),"."," ")))</f>
         <v>i guess women are really more social these days finding so many fun things to do outside</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" t="s">
+        <v>12</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="2" t="s">
         <v>1060</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" t="s">
-        <v>12</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>1061</v>
       </c>
       <c r="K66" t="s">
         <v>12</v>
@@ -8263,7 +8247,7 @@
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>235</v>
@@ -8320,7 +8304,7 @@
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>239</v>
@@ -8434,7 +8418,7 @@
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>247</v>
@@ -8548,7 +8532,7 @@
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C72" t="s">
         <v>255</v>
@@ -8662,7 +8646,7 @@
     </row>
     <row r="74" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>263</v>
@@ -8719,7 +8703,7 @@
     </row>
     <row r="75" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>267</v>
@@ -8833,7 +8817,7 @@
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>273</v>
@@ -8893,44 +8877,44 @@
         <v>875</v>
       </c>
       <c r="C78" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
         <v>i was going to catch a great buy live a life of celebrity whered it all go wrong</v>
       </c>
       <c r="E78" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" t="s">
+        <v>12</v>
+      </c>
+      <c r="I78" t="s">
+        <v>12</v>
+      </c>
+      <c r="J78" t="s">
+        <v>1179</v>
+      </c>
+      <c r="K78" t="s">
+        <v>12</v>
+      </c>
+      <c r="L78" t="s">
+        <v>12</v>
+      </c>
+      <c r="M78" t="s">
+        <v>12</v>
+      </c>
+      <c r="N78" t="s">
+        <v>12</v>
+      </c>
+      <c r="O78" t="s">
         <v>1180</v>
-      </c>
-      <c r="F78" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H78" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" t="s">
-        <v>12</v>
-      </c>
-      <c r="J78" t="s">
-        <v>1181</v>
-      </c>
-      <c r="K78" t="s">
-        <v>12</v>
-      </c>
-      <c r="L78" t="s">
-        <v>12</v>
-      </c>
-      <c r="M78" t="s">
-        <v>12</v>
-      </c>
-      <c r="N78" t="s">
-        <v>12</v>
-      </c>
-      <c r="O78" t="s">
-        <v>1182</v>
       </c>
       <c r="P78" t="s">
         <v>12</v>
@@ -8947,7 +8931,7 @@
     </row>
     <row r="79" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>277</v>
@@ -9064,7 +9048,7 @@
         <v>121</v>
       </c>
       <c r="B81" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>289</v>
@@ -9121,7 +9105,7 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>285</v>
@@ -9178,7 +9162,7 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>293</v>
@@ -9235,7 +9219,7 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>297</v>
@@ -9292,7 +9276,7 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>301</v>
@@ -9349,7 +9333,7 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>305</v>
@@ -9406,7 +9390,7 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>309</v>
@@ -9463,7 +9447,7 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>313</v>
@@ -9691,7 +9675,7 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B92" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>329</v>
@@ -9748,7 +9732,7 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>333</v>
@@ -9805,47 +9789,47 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="1"/>
         <v>ill let you kill me but first i want you to do something fun for me before that</v>
       </c>
       <c r="E94" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>12</v>
+      </c>
+      <c r="J94" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="F94" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" t="s">
-        <v>12</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" t="s">
-        <v>12</v>
-      </c>
-      <c r="J94" s="2" t="s">
+      <c r="K94" t="s">
+        <v>12</v>
+      </c>
+      <c r="L94" t="s">
+        <v>12</v>
+      </c>
+      <c r="M94" t="s">
+        <v>12</v>
+      </c>
+      <c r="N94" t="s">
+        <v>12</v>
+      </c>
+      <c r="O94" s="2" t="s">
         <v>1100</v>
-      </c>
-      <c r="K94" t="s">
-        <v>12</v>
-      </c>
-      <c r="L94" t="s">
-        <v>12</v>
-      </c>
-      <c r="M94" t="s">
-        <v>12</v>
-      </c>
-      <c r="N94" t="s">
-        <v>12</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>1101</v>
       </c>
       <c r="P94" s="2" t="s">
         <v>14</v>
@@ -9919,7 +9903,7 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>341</v>
@@ -9976,7 +9960,7 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>345</v>
@@ -10033,7 +10017,7 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>857</v>
@@ -10150,7 +10134,7 @@
         <v>22</v>
       </c>
       <c r="B100" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>354</v>
@@ -10267,14 +10251,14 @@
         <v>965</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="1"/>
         <v>im so sleepy ho i just want you to leave me alone</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>13</v>
@@ -10289,22 +10273,22 @@
         <v>12</v>
       </c>
       <c r="J102" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K102" t="s">
+        <v>12</v>
+      </c>
+      <c r="L102" t="s">
+        <v>12</v>
+      </c>
+      <c r="M102" t="s">
+        <v>12</v>
+      </c>
+      <c r="N102" t="s">
+        <v>12</v>
+      </c>
+      <c r="O102" s="2" t="s">
         <v>1065</v>
-      </c>
-      <c r="K102" t="s">
-        <v>12</v>
-      </c>
-      <c r="L102" t="s">
-        <v>12</v>
-      </c>
-      <c r="M102" t="s">
-        <v>12</v>
-      </c>
-      <c r="N102" t="s">
-        <v>12</v>
-      </c>
-      <c r="O102" s="2" t="s">
-        <v>1066</v>
       </c>
       <c r="P102" t="s">
         <v>12</v>
@@ -10321,7 +10305,7 @@
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C103" t="s">
         <v>360</v>
@@ -10378,7 +10362,7 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>364</v>
@@ -10435,7 +10419,7 @@
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>368</v>
@@ -10492,7 +10476,7 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B106" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C106" t="s">
         <v>371</v>
@@ -10549,7 +10533,7 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B107" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>375</v>
@@ -10663,7 +10647,7 @@
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>383</v>
@@ -10720,7 +10704,7 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B110" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>385</v>
@@ -10777,17 +10761,17 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="C111" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="1"/>
         <v>is it ok if i get mad right now</v>
       </c>
       <c r="E111" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
@@ -10817,7 +10801,7 @@
         <v>12</v>
       </c>
       <c r="O111" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="P111" t="s">
         <v>12</v>
@@ -10834,7 +10818,7 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>388</v>
@@ -10948,7 +10932,7 @@
     </row>
     <row r="114" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>396</v>
@@ -11005,7 +10989,7 @@
     </row>
     <row r="115" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>400</v>
@@ -11062,7 +11046,7 @@
     </row>
     <row r="116" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>403</v>
@@ -11176,7 +11160,7 @@
     </row>
     <row r="118" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>409</v>
@@ -11290,7 +11274,7 @@
     </row>
     <row r="120" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B120" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>876</v>
@@ -11347,7 +11331,7 @@
     </row>
     <row r="121" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>420</v>
@@ -11404,7 +11388,7 @@
     </row>
     <row r="122" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B122" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>424</v>
@@ -11461,7 +11445,7 @@
     </row>
     <row r="123" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>428</v>
@@ -11518,7 +11502,7 @@
     </row>
     <row r="124" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>432</v>
@@ -11632,7 +11616,7 @@
     </row>
     <row r="126" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B126" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>439</v>
@@ -11689,7 +11673,7 @@
     </row>
     <row r="127" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B127" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>442</v>
@@ -11746,7 +11730,7 @@
     </row>
     <row r="128" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>445</v>
@@ -11917,7 +11901,7 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B131" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>449</v>
@@ -11974,7 +11958,7 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B132" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>461</v>
@@ -12031,7 +12015,7 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B133" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>465</v>
@@ -12145,7 +12129,7 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B135" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>473</v>
@@ -12202,7 +12186,7 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B136" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>477</v>
@@ -12316,7 +12300,7 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B138" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>485</v>
@@ -12373,7 +12357,7 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>489</v>
@@ -12430,7 +12414,7 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B140" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>493</v>
@@ -12487,7 +12471,7 @@
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>497</v>
@@ -12658,47 +12642,47 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D144" t="str">
         <f t="shared" si="2"/>
         <v>now people dont even know who lives next door to them shouldnt we know our neighbors better</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H144" t="s">
+        <v>12</v>
+      </c>
+      <c r="I144" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J144" t="s">
         <v>1080</v>
       </c>
-      <c r="F144" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H144" t="s">
-        <v>12</v>
-      </c>
-      <c r="I144" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J144" t="s">
+      <c r="K144" t="s">
+        <v>12</v>
+      </c>
+      <c r="L144" t="s">
+        <v>12</v>
+      </c>
+      <c r="M144" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N144" t="s">
+        <v>12</v>
+      </c>
+      <c r="O144" t="s">
         <v>1081</v>
-      </c>
-      <c r="K144" t="s">
-        <v>12</v>
-      </c>
-      <c r="L144" t="s">
-        <v>12</v>
-      </c>
-      <c r="M144" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N144" t="s">
-        <v>12</v>
-      </c>
-      <c r="O144" t="s">
-        <v>1082</v>
       </c>
       <c r="P144" t="s">
         <v>12</v>
@@ -12715,7 +12699,7 @@
     </row>
     <row r="145" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B145" t="s">
-        <v>969</v>
+        <v>1188</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>506</v>
@@ -12739,7 +12723,7 @@
       <c r="I145" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J145" t="s">
+      <c r="J145" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K145" t="s">
@@ -12748,8 +12732,8 @@
       <c r="L145" t="s">
         <v>12</v>
       </c>
-      <c r="M145" t="s">
-        <v>12</v>
+      <c r="M145" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="N145" t="s">
         <v>12</v>
@@ -12772,7 +12756,7 @@
     </row>
     <row r="146" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B146" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>507</v>
@@ -12886,7 +12870,7 @@
     </row>
     <row r="148" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B148" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>511</v>
@@ -12943,7 +12927,7 @@
     </row>
     <row r="149" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B149" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>514</v>
@@ -13000,7 +12984,7 @@
     </row>
     <row r="150" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B150" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>518</v>
@@ -13114,7 +13098,7 @@
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B152" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>526</v>
@@ -13171,7 +13155,7 @@
     </row>
     <row r="153" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B153" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>529</v>
@@ -13228,7 +13212,7 @@
     </row>
     <row r="154" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B154" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>533</v>
@@ -13342,7 +13326,7 @@
     </row>
     <row r="156" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B156" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>541</v>
@@ -13402,44 +13386,44 @@
         <v>891</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D157" t="str">
         <f t="shared" si="2"/>
         <v>some old people refuse to make use of special seats reserved for the elderly what do you think of that</v>
       </c>
       <c r="E157" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F157" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" t="s">
+        <v>12</v>
+      </c>
+      <c r="H157" t="s">
+        <v>12</v>
+      </c>
+      <c r="I157" t="s">
+        <v>12</v>
+      </c>
+      <c r="J157" s="2" t="s">
         <v>1025</v>
       </c>
-      <c r="F157" t="s">
-        <v>12</v>
-      </c>
-      <c r="G157" t="s">
-        <v>12</v>
-      </c>
-      <c r="H157" t="s">
-        <v>12</v>
-      </c>
-      <c r="I157" t="s">
-        <v>12</v>
-      </c>
-      <c r="J157" s="2" t="s">
+      <c r="K157" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L157" t="s">
+        <v>12</v>
+      </c>
+      <c r="M157" t="s">
+        <v>12</v>
+      </c>
+      <c r="N157" t="s">
+        <v>12</v>
+      </c>
+      <c r="O157" s="2" t="s">
         <v>1026</v>
-      </c>
-      <c r="K157" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L157" t="s">
-        <v>12</v>
-      </c>
-      <c r="M157" t="s">
-        <v>12</v>
-      </c>
-      <c r="N157" t="s">
-        <v>12</v>
-      </c>
-      <c r="O157" s="2" t="s">
-        <v>1027</v>
       </c>
       <c r="P157" t="s">
         <v>12</v>
@@ -13456,7 +13440,7 @@
     </row>
     <row r="158" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B158" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>545</v>
@@ -13570,7 +13554,7 @@
     </row>
     <row r="160" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B160" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>553</v>
@@ -13627,7 +13611,7 @@
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B161" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>556</v>
@@ -13684,7 +13668,7 @@
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B162" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>559</v>
@@ -13744,14 +13728,14 @@
         <v>862</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="2"/>
         <v>that is to say we are brothers there is no reason for us to fight</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="F163" t="s">
         <v>12</v>
@@ -13766,7 +13750,7 @@
         <v>12</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="K163" t="s">
         <v>12</v>
@@ -13781,7 +13765,7 @@
         <v>12</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="P163" t="s">
         <v>12</v>
@@ -13798,7 +13782,7 @@
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B164" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>563</v>
@@ -13855,7 +13839,7 @@
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B165" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>567</v>
@@ -13912,7 +13896,7 @@
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B166" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>863</v>
@@ -14026,10 +14010,10 @@
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B168" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="2"/>
@@ -14083,7 +14067,7 @@
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B169" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>934</v>
@@ -14114,7 +14098,7 @@
         <v>12</v>
       </c>
       <c r="L169" s="5" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M169" t="s">
         <v>12</v>
@@ -14140,7 +14124,7 @@
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B170" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>578</v>
@@ -14197,10 +14181,10 @@
     </row>
     <row r="171" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B171" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="2"/>
@@ -14254,7 +14238,7 @@
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B172" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>585</v>
@@ -14311,10 +14295,10 @@
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B173" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D173" t="str">
         <f t="shared" si="2"/>
@@ -14368,7 +14352,7 @@
     </row>
     <row r="174" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B174" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>590</v>
@@ -14599,32 +14583,32 @@
     </row>
     <row r="178" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D178" t="str">
         <f t="shared" si="2"/>
         <v>to tell you the hee truth this is all an act ho what do you think im really like ho</v>
       </c>
       <c r="E178" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" t="s">
+        <v>12</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I178" t="s">
+        <v>12</v>
+      </c>
+      <c r="J178" s="2" t="s">
         <v>1013</v>
-      </c>
-      <c r="F178" t="s">
-        <v>12</v>
-      </c>
-      <c r="G178" t="s">
-        <v>12</v>
-      </c>
-      <c r="H178" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I178" t="s">
-        <v>12</v>
-      </c>
-      <c r="J178" s="2" t="s">
-        <v>1014</v>
       </c>
       <c r="K178" t="s">
         <v>12</v>
@@ -14656,7 +14640,7 @@
     </row>
     <row r="179" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>893</v>
@@ -14773,7 +14757,7 @@
     </row>
     <row r="181" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B181" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>609</v>
@@ -14830,7 +14814,7 @@
     </row>
     <row r="182" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>613</v>
@@ -14887,7 +14871,7 @@
     </row>
     <row r="183" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B183" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>616</v>
@@ -14944,7 +14928,7 @@
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B184" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>623</v>
@@ -15004,7 +14988,7 @@
         <v>121</v>
       </c>
       <c r="B185" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>627</v>
@@ -15061,7 +15045,7 @@
     </row>
     <row r="186" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B186" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>851</v>
@@ -15118,10 +15102,10 @@
     </row>
     <row r="187" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D187" t="str">
         <f t="shared" si="2"/>
@@ -15175,7 +15159,7 @@
     </row>
     <row r="188" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>635</v>
@@ -15289,7 +15273,7 @@
     </row>
     <row r="190" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B190" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>652</v>
@@ -15346,7 +15330,7 @@
     </row>
     <row r="191" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B191" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>643</v>
@@ -15517,7 +15501,7 @@
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B194" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>884</v>
@@ -15557,7 +15541,7 @@
         <v>12</v>
       </c>
       <c r="O194" s="2" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="P194" t="s">
         <v>12</v>
@@ -15574,7 +15558,7 @@
     </row>
     <row r="195" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B195" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>656</v>
@@ -15691,7 +15675,7 @@
         <v>121</v>
       </c>
       <c r="B197" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>928</v>
@@ -15748,7 +15732,7 @@
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B198" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>663</v>
@@ -15805,7 +15789,7 @@
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B199" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>667</v>
@@ -15862,7 +15846,7 @@
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B200" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>671</v>
@@ -15872,7 +15856,7 @@
         <v>what should i wear</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="F200" t="s">
         <v>12</v>
@@ -15919,7 +15903,7 @@
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B201" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>674</v>
@@ -16033,7 +16017,7 @@
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B203" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>682</v>
@@ -16090,7 +16074,7 @@
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B204" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>686</v>
@@ -16147,7 +16131,7 @@
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B205" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>690</v>
@@ -16318,47 +16302,47 @@
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="D208" t="str">
         <f t="shared" si="3"/>
         <v>when it came right down to it you couldnt do anything to me</v>
       </c>
       <c r="E208" s="2" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F208" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" t="s">
+        <v>12</v>
+      </c>
+      <c r="H208" t="s">
+        <v>12</v>
+      </c>
+      <c r="I208" t="s">
+        <v>12</v>
+      </c>
+      <c r="J208" s="2" t="s">
+        <v>1171</v>
+      </c>
+      <c r="K208" t="s">
+        <v>12</v>
+      </c>
+      <c r="L208" t="s">
+        <v>12</v>
+      </c>
+      <c r="M208" t="s">
+        <v>12</v>
+      </c>
+      <c r="N208" t="s">
+        <v>12</v>
+      </c>
+      <c r="O208" s="2" t="s">
         <v>1172</v>
-      </c>
-      <c r="F208" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" t="s">
-        <v>12</v>
-      </c>
-      <c r="H208" t="s">
-        <v>12</v>
-      </c>
-      <c r="I208" t="s">
-        <v>12</v>
-      </c>
-      <c r="J208" s="2" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K208" t="s">
-        <v>12</v>
-      </c>
-      <c r="L208" t="s">
-        <v>12</v>
-      </c>
-      <c r="M208" t="s">
-        <v>12</v>
-      </c>
-      <c r="N208" t="s">
-        <v>12</v>
-      </c>
-      <c r="O208" s="2" t="s">
-        <v>1174</v>
       </c>
       <c r="P208" t="s">
         <v>12</v>
@@ -16603,7 +16587,7 @@
     </row>
     <row r="213" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B213" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>714</v>
@@ -16663,7 +16647,7 @@
         <v>911</v>
       </c>
       <c r="C214" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="D214" t="str">
         <f t="shared" si="3"/>
@@ -16714,7 +16698,7 @@
     </row>
     <row r="215" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B215" t="s">
-        <v>1148</v>
+        <v>1072</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>901</v>
@@ -16747,8 +16731,8 @@
       <c r="L215" t="s">
         <v>12</v>
       </c>
-      <c r="M215" t="s">
-        <v>12</v>
+      <c r="M215" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="N215" s="2" t="s">
         <v>13</v>
@@ -16771,7 +16755,7 @@
     </row>
     <row r="216" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B216" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>852</v>
@@ -16828,7 +16812,7 @@
     </row>
     <row r="217" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B217" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>720</v>
@@ -16885,7 +16869,7 @@
     </row>
     <row r="218" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B218" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>724</v>
@@ -16942,7 +16926,7 @@
     </row>
     <row r="219" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B219" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>728</v>
@@ -17056,7 +17040,7 @@
     </row>
     <row r="221" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B221" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>736</v>
@@ -17113,7 +17097,7 @@
     </row>
     <row r="222" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B222" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>740</v>
@@ -17170,7 +17154,7 @@
     </row>
     <row r="223" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B223" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>744</v>
@@ -17230,7 +17214,7 @@
         <v>22</v>
       </c>
       <c r="B224" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>910</v>
@@ -17287,17 +17271,17 @@
     </row>
     <row r="225" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D225" t="str">
         <f t="shared" si="3"/>
         <v>would you be willing to spend time and money to see people you havent contacted for years</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F225" t="s">
         <v>12</v>
@@ -17312,7 +17296,7 @@
         <v>12</v>
       </c>
       <c r="J225" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="K225" t="s">
         <v>12</v>
@@ -17327,7 +17311,7 @@
         <v>12</v>
       </c>
       <c r="O225" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P225" t="s">
         <v>12</v>
@@ -17344,7 +17328,7 @@
     </row>
     <row r="226" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B226" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>751</v>
@@ -17404,7 +17388,7 @@
         <v>22</v>
       </c>
       <c r="B227" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>755</v>
@@ -17518,7 +17502,7 @@
     </row>
     <row r="229" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B229" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>763</v>
@@ -17575,7 +17559,7 @@
     </row>
     <row r="230" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B230" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>767</v>
@@ -17632,7 +17616,7 @@
     </row>
     <row r="231" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B231" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>770</v>
@@ -17746,7 +17730,7 @@
     </row>
     <row r="233" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B233" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>774</v>
@@ -17803,7 +17787,7 @@
     </row>
     <row r="234" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B234" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>777</v>
@@ -17860,7 +17844,7 @@
     </row>
     <row r="235" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B235" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>781</v>
@@ -17977,7 +17961,7 @@
         <v>862</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D237" t="str">
         <f t="shared" si="3"/>
@@ -17999,7 +17983,7 @@
         <v>12</v>
       </c>
       <c r="J237" s="2" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="K237" t="s">
         <v>12</v>
@@ -18031,7 +18015,7 @@
     </row>
     <row r="238" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B238" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>789</v>
@@ -18091,7 +18075,7 @@
         <v>950</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D239" t="str">
         <f t="shared" si="3"/>
@@ -18145,7 +18129,7 @@
     </row>
     <row r="240" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B240" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>796</v>
@@ -18154,10 +18138,10 @@
         <f t="shared" si="3"/>
         <v>you however are talking to me right here are you the exception to this rule</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E240" s="2" t="s">
         <v>797</v>
       </c>
-      <c r="F240" t="s">
+      <c r="F240" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G240" t="s">
@@ -18202,7 +18186,7 @@
     </row>
     <row r="241" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B241" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>799</v>
@@ -18430,7 +18414,7 @@
     </row>
     <row r="245" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B245" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>814</v>
@@ -18487,7 +18471,7 @@
     </row>
     <row r="246" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B246" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>897</v>
@@ -18601,7 +18585,7 @@
     </row>
     <row r="248" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B248" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>820</v>
@@ -18658,10 +18642,10 @@
     </row>
     <row r="249" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B249" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D249" t="str">
         <f t="shared" si="3"/>
@@ -18698,7 +18682,7 @@
         <v>12</v>
       </c>
       <c r="O249" s="2" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="P249" s="2" t="s">
         <v>16</v>
@@ -18715,7 +18699,7 @@
     </row>
     <row r="250" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C250" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D250" t="str">
         <f t="shared" si="3"/>
@@ -18737,22 +18721,22 @@
         <v>12</v>
       </c>
       <c r="J250" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K250" t="s">
+        <v>12</v>
+      </c>
+      <c r="L250" t="s">
+        <v>12</v>
+      </c>
+      <c r="M250" t="s">
+        <v>12</v>
+      </c>
+      <c r="N250" t="s">
+        <v>12</v>
+      </c>
+      <c r="O250" s="2" t="s">
         <v>1105</v>
-      </c>
-      <c r="K250" t="s">
-        <v>12</v>
-      </c>
-      <c r="L250" t="s">
-        <v>12</v>
-      </c>
-      <c r="M250" t="s">
-        <v>12</v>
-      </c>
-      <c r="N250" t="s">
-        <v>12</v>
-      </c>
-      <c r="O250" s="2" t="s">
-        <v>1106</v>
       </c>
       <c r="P250" t="s">
         <v>12</v>
@@ -18826,17 +18810,17 @@
     </row>
     <row r="252" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B252" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D252" t="str">
         <f t="shared" si="3"/>
         <v>youll have a bleak future if you spend too much time running around pretending to be a phantom thief</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F252" s="2" t="s">
         <v>13</v>
@@ -18866,7 +18850,7 @@
         <v>12</v>
       </c>
       <c r="O252" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P252" t="s">
         <v>12</v>
@@ -18940,7 +18924,7 @@
     </row>
     <row r="254" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B254" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>829</v>
@@ -18997,7 +18981,7 @@
     </row>
     <row r="255" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B255" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>853</v>
@@ -19054,7 +19038,7 @@
     </row>
     <row r="256" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B256" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>832</v>
@@ -19225,7 +19209,7 @@
     </row>
     <row r="259" spans="2:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B259" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>842</v>

</xml_diff>